<commit_message>
Add data and data import adjustments
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\HYPERracing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71450409-61AE-4BE8-80BD-2E32376DAAA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86F845C-B799-494B-9444-5FE05C141906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="drivers" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1261" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1751" uniqueCount="113">
   <si>
     <t>Driver</t>
   </si>
@@ -344,12 +344,33 @@
   <si>
     <t>A. Dembele</t>
   </si>
+  <si>
+    <t>RuizMotorsport</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>T. Leclere</t>
+  </si>
+  <si>
+    <t>L. Steward</t>
+  </si>
+  <si>
+    <t>G. Almeida</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>W. Dilshat</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -375,6 +396,13 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -404,11 +432,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -627,10 +656,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -857,6 +886,38 @@
       </c>
       <c r="B28" s="1" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -869,10 +930,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F361"/>
+  <dimension ref="A1:F521"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G360" sqref="G360"/>
+    <sheetView tabSelected="1" topLeftCell="A501" workbookViewId="0">
+      <selection activeCell="E521" sqref="E521:F521"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8100,9 +8161,3210 @@
         <v>45</v>
       </c>
     </row>
+    <row r="362" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A362" s="1">
+        <v>2</v>
+      </c>
+      <c r="B362" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C362" s="1">
+        <v>1</v>
+      </c>
+      <c r="D362" s="1">
+        <v>0</v>
+      </c>
+      <c r="E362" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F362" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="363" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A363" s="1">
+        <v>2</v>
+      </c>
+      <c r="B363" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C363" s="1">
+        <v>2</v>
+      </c>
+      <c r="D363" s="1">
+        <v>0</v>
+      </c>
+      <c r="E363" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F363" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="364" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A364" s="1">
+        <v>2</v>
+      </c>
+      <c r="B364" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C364" s="1">
+        <v>3</v>
+      </c>
+      <c r="D364" s="1">
+        <v>0</v>
+      </c>
+      <c r="E364" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F364" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="365" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A365" s="1">
+        <v>2</v>
+      </c>
+      <c r="B365" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C365" s="1">
+        <v>4</v>
+      </c>
+      <c r="D365" s="1">
+        <v>0</v>
+      </c>
+      <c r="E365" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F365" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="366" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A366" s="1">
+        <v>2</v>
+      </c>
+      <c r="B366" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C366" s="1">
+        <v>5</v>
+      </c>
+      <c r="D366" s="1">
+        <v>0</v>
+      </c>
+      <c r="E366" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F366" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="367" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A367" s="1">
+        <v>2</v>
+      </c>
+      <c r="B367" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C367" s="1">
+        <v>6</v>
+      </c>
+      <c r="D367" s="1">
+        <v>0</v>
+      </c>
+      <c r="E367" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F367" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="368" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A368" s="1">
+        <v>2</v>
+      </c>
+      <c r="B368" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C368" s="1">
+        <v>7</v>
+      </c>
+      <c r="D368" s="1">
+        <v>1</v>
+      </c>
+      <c r="E368" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F368" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="369" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A369" s="1">
+        <v>2</v>
+      </c>
+      <c r="B369" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C369" s="1">
+        <v>8</v>
+      </c>
+      <c r="D369" s="1">
+        <v>0</v>
+      </c>
+      <c r="E369" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F369" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="370" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A370" s="1">
+        <v>2</v>
+      </c>
+      <c r="B370" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C370" s="1">
+        <v>9</v>
+      </c>
+      <c r="D370" s="1">
+        <v>0</v>
+      </c>
+      <c r="E370" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F370" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="371" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A371" s="1">
+        <v>2</v>
+      </c>
+      <c r="B371" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C371" s="1">
+        <v>10</v>
+      </c>
+      <c r="D371" s="1">
+        <v>0</v>
+      </c>
+      <c r="E371" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F371" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="372" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A372" s="1">
+        <v>2</v>
+      </c>
+      <c r="B372" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C372" s="1">
+        <v>11</v>
+      </c>
+      <c r="D372" s="1">
+        <v>0</v>
+      </c>
+      <c r="E372" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F372" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="373" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A373" s="1">
+        <v>2</v>
+      </c>
+      <c r="B373" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C373" s="1">
+        <v>12</v>
+      </c>
+      <c r="D373" s="1">
+        <v>0</v>
+      </c>
+      <c r="E373" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F373" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="374" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A374" s="1">
+        <v>2</v>
+      </c>
+      <c r="B374" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C374" s="1">
+        <v>13</v>
+      </c>
+      <c r="D374" s="1">
+        <v>0</v>
+      </c>
+      <c r="E374" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F374" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="375" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A375" s="1">
+        <v>2</v>
+      </c>
+      <c r="B375" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C375" s="1">
+        <v>14</v>
+      </c>
+      <c r="D375" s="1">
+        <v>0</v>
+      </c>
+      <c r="E375" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F375" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="376" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A376" s="1">
+        <v>2</v>
+      </c>
+      <c r="B376" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C376" s="1">
+        <v>15</v>
+      </c>
+      <c r="D376" s="1">
+        <v>0</v>
+      </c>
+      <c r="E376" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F376" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="377" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A377" s="1">
+        <v>2</v>
+      </c>
+      <c r="B377" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C377" s="1">
+        <v>16</v>
+      </c>
+      <c r="D377" s="1">
+        <v>0</v>
+      </c>
+      <c r="E377" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F377" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="378" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A378" s="1">
+        <v>2</v>
+      </c>
+      <c r="B378" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C378" s="1">
+        <v>17</v>
+      </c>
+      <c r="D378" s="1">
+        <v>0</v>
+      </c>
+      <c r="E378" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F378" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="379" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A379" s="1">
+        <v>2</v>
+      </c>
+      <c r="B379" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C379" s="1">
+        <v>18</v>
+      </c>
+      <c r="D379" s="1">
+        <v>0</v>
+      </c>
+      <c r="E379" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F379" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="380" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A380" s="1">
+        <v>2</v>
+      </c>
+      <c r="B380" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C380" s="1">
+        <v>19</v>
+      </c>
+      <c r="D380" s="1">
+        <v>0</v>
+      </c>
+      <c r="E380" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F380" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="381" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A381" s="1">
+        <v>2</v>
+      </c>
+      <c r="B381" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C381" s="1">
+        <v>20</v>
+      </c>
+      <c r="D381" s="1">
+        <v>0</v>
+      </c>
+      <c r="E381" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F381" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="382" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A382" s="1">
+        <v>2</v>
+      </c>
+      <c r="B382" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C382" s="1">
+        <v>1</v>
+      </c>
+      <c r="D382" s="1">
+        <v>0</v>
+      </c>
+      <c r="E382" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F382" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="383" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A383" s="1">
+        <v>2</v>
+      </c>
+      <c r="B383" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C383" s="1">
+        <v>2</v>
+      </c>
+      <c r="D383" s="1">
+        <v>0</v>
+      </c>
+      <c r="E383" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F383" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="384" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A384" s="1">
+        <v>2</v>
+      </c>
+      <c r="B384" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C384" s="1">
+        <v>3</v>
+      </c>
+      <c r="D384" s="1">
+        <v>0</v>
+      </c>
+      <c r="E384" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F384" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="385" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A385" s="1">
+        <v>2</v>
+      </c>
+      <c r="B385" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C385" s="1">
+        <v>4</v>
+      </c>
+      <c r="D385" s="1">
+        <v>0</v>
+      </c>
+      <c r="E385" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F385" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="386" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A386" s="1">
+        <v>2</v>
+      </c>
+      <c r="B386" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C386" s="1">
+        <v>5</v>
+      </c>
+      <c r="D386" s="1">
+        <v>0</v>
+      </c>
+      <c r="E386" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F386" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="387" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A387" s="1">
+        <v>2</v>
+      </c>
+      <c r="B387" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C387" s="1">
+        <v>6</v>
+      </c>
+      <c r="D387" s="1">
+        <v>0</v>
+      </c>
+      <c r="E387" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F387" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="388" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A388" s="1">
+        <v>2</v>
+      </c>
+      <c r="B388" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C388" s="1">
+        <v>7</v>
+      </c>
+      <c r="D388" s="1">
+        <v>0</v>
+      </c>
+      <c r="E388" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F388" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="389" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A389" s="1">
+        <v>2</v>
+      </c>
+      <c r="B389" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C389" s="1">
+        <v>8</v>
+      </c>
+      <c r="D389" s="1">
+        <v>0</v>
+      </c>
+      <c r="E389" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F389" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="390" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A390" s="1">
+        <v>2</v>
+      </c>
+      <c r="B390" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C390" s="1">
+        <v>9</v>
+      </c>
+      <c r="D390" s="1">
+        <v>0</v>
+      </c>
+      <c r="E390" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F390" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="391" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A391" s="1">
+        <v>2</v>
+      </c>
+      <c r="B391" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C391" s="1">
+        <v>10</v>
+      </c>
+      <c r="D391" s="1">
+        <v>0</v>
+      </c>
+      <c r="E391" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F391" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="392" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A392" s="1">
+        <v>2</v>
+      </c>
+      <c r="B392" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C392" s="1">
+        <v>11</v>
+      </c>
+      <c r="D392" s="1">
+        <v>0</v>
+      </c>
+      <c r="E392" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F392" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="393" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A393" s="1">
+        <v>2</v>
+      </c>
+      <c r="B393" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C393" s="1">
+        <v>12</v>
+      </c>
+      <c r="D393" s="1">
+        <v>0</v>
+      </c>
+      <c r="E393" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F393" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="394" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A394" s="1">
+        <v>2</v>
+      </c>
+      <c r="B394" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C394" s="1">
+        <v>13</v>
+      </c>
+      <c r="D394" s="1">
+        <v>0</v>
+      </c>
+      <c r="E394" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F394" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="395" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A395" s="1">
+        <v>2</v>
+      </c>
+      <c r="B395" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C395" s="1">
+        <v>14</v>
+      </c>
+      <c r="D395" s="1">
+        <v>0</v>
+      </c>
+      <c r="E395" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F395" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="396" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A396" s="1">
+        <v>2</v>
+      </c>
+      <c r="B396" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C396" s="1">
+        <v>15</v>
+      </c>
+      <c r="D396" s="1">
+        <v>0</v>
+      </c>
+      <c r="E396" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F396" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="397" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A397" s="1">
+        <v>2</v>
+      </c>
+      <c r="B397" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C397" s="1">
+        <v>16</v>
+      </c>
+      <c r="D397" s="1">
+        <v>0</v>
+      </c>
+      <c r="E397" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F397" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="398" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A398" s="1">
+        <v>2</v>
+      </c>
+      <c r="B398" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C398" s="1">
+        <v>17</v>
+      </c>
+      <c r="D398" s="1">
+        <v>0</v>
+      </c>
+      <c r="E398" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F398" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="399" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A399" s="1">
+        <v>2</v>
+      </c>
+      <c r="B399" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C399" s="1">
+        <v>18</v>
+      </c>
+      <c r="D399" s="1">
+        <v>0</v>
+      </c>
+      <c r="E399" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F399" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="400" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A400" s="1">
+        <v>2</v>
+      </c>
+      <c r="B400" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C400" s="1">
+        <v>19</v>
+      </c>
+      <c r="D400" s="1">
+        <v>0</v>
+      </c>
+      <c r="E400" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F400" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="401" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A401" s="1">
+        <v>2</v>
+      </c>
+      <c r="B401" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C401" s="1">
+        <v>20</v>
+      </c>
+      <c r="D401" s="1">
+        <v>1</v>
+      </c>
+      <c r="E401" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F401" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="402" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A402" s="1">
+        <v>3</v>
+      </c>
+      <c r="B402" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C402" s="1">
+        <v>1</v>
+      </c>
+      <c r="D402" s="1">
+        <v>0</v>
+      </c>
+      <c r="E402" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F402" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="403" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A403" s="1">
+        <v>3</v>
+      </c>
+      <c r="B403" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C403" s="1">
+        <v>2</v>
+      </c>
+      <c r="D403" s="1">
+        <v>0</v>
+      </c>
+      <c r="E403" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F403" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="404" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A404" s="1">
+        <v>3</v>
+      </c>
+      <c r="B404" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C404" s="1">
+        <v>3</v>
+      </c>
+      <c r="D404" s="1">
+        <v>0</v>
+      </c>
+      <c r="E404" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F404" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="405" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A405" s="1">
+        <v>3</v>
+      </c>
+      <c r="B405" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C405" s="1">
+        <v>4</v>
+      </c>
+      <c r="D405" s="1">
+        <v>0</v>
+      </c>
+      <c r="E405" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F405" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="406" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A406" s="1">
+        <v>3</v>
+      </c>
+      <c r="B406" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C406" s="1">
+        <v>5</v>
+      </c>
+      <c r="D406" s="1">
+        <v>0</v>
+      </c>
+      <c r="E406" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F406" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="407" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A407" s="1">
+        <v>3</v>
+      </c>
+      <c r="B407" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C407" s="1">
+        <v>6</v>
+      </c>
+      <c r="D407" s="1">
+        <v>0</v>
+      </c>
+      <c r="E407" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F407" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="408" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A408" s="1">
+        <v>3</v>
+      </c>
+      <c r="B408" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C408" s="1">
+        <v>7</v>
+      </c>
+      <c r="D408" s="1">
+        <v>0</v>
+      </c>
+      <c r="E408" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F408" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="409" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A409" s="1">
+        <v>3</v>
+      </c>
+      <c r="B409" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C409" s="1">
+        <v>8</v>
+      </c>
+      <c r="D409" s="1">
+        <v>0</v>
+      </c>
+      <c r="E409" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F409" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="410" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A410" s="1">
+        <v>3</v>
+      </c>
+      <c r="B410" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C410" s="1">
+        <v>9</v>
+      </c>
+      <c r="D410" s="1">
+        <v>0</v>
+      </c>
+      <c r="E410" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F410" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="411" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A411" s="1">
+        <v>3</v>
+      </c>
+      <c r="B411" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C411" s="1">
+        <v>10</v>
+      </c>
+      <c r="D411" s="1">
+        <v>0</v>
+      </c>
+      <c r="E411" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F411" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="412" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A412" s="1">
+        <v>3</v>
+      </c>
+      <c r="B412" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C412" s="1">
+        <v>11</v>
+      </c>
+      <c r="D412" s="1">
+        <v>0</v>
+      </c>
+      <c r="E412" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F412" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="413" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A413" s="1">
+        <v>3</v>
+      </c>
+      <c r="B413" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C413" s="1">
+        <v>12</v>
+      </c>
+      <c r="D413" s="1">
+        <v>0</v>
+      </c>
+      <c r="E413" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F413" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="414" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A414" s="1">
+        <v>3</v>
+      </c>
+      <c r="B414" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C414" s="1">
+        <v>13</v>
+      </c>
+      <c r="D414" s="1">
+        <v>0</v>
+      </c>
+      <c r="E414" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F414" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="415" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A415" s="1">
+        <v>3</v>
+      </c>
+      <c r="B415" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C415" s="1">
+        <v>14</v>
+      </c>
+      <c r="D415" s="1">
+        <v>0</v>
+      </c>
+      <c r="E415" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F415" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="416" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A416" s="1">
+        <v>3</v>
+      </c>
+      <c r="B416" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C416" s="1">
+        <v>15</v>
+      </c>
+      <c r="D416" s="1">
+        <v>1</v>
+      </c>
+      <c r="E416" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F416" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="417" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A417" s="1">
+        <v>3</v>
+      </c>
+      <c r="B417" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C417" s="1">
+        <v>16</v>
+      </c>
+      <c r="D417" s="1">
+        <v>0</v>
+      </c>
+      <c r="E417" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F417" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="418" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A418" s="1">
+        <v>3</v>
+      </c>
+      <c r="B418" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C418" s="1">
+        <v>17</v>
+      </c>
+      <c r="D418" s="1">
+        <v>0</v>
+      </c>
+      <c r="E418" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F418" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="419" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A419" s="1">
+        <v>3</v>
+      </c>
+      <c r="B419" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C419" s="1">
+        <v>18</v>
+      </c>
+      <c r="D419" s="1">
+        <v>0</v>
+      </c>
+      <c r="E419" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F419" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="420" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A420" s="1">
+        <v>3</v>
+      </c>
+      <c r="B420" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C420" s="1">
+        <v>19</v>
+      </c>
+      <c r="D420" s="1">
+        <v>0</v>
+      </c>
+      <c r="E420" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F420" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="421" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A421" s="1">
+        <v>3</v>
+      </c>
+      <c r="B421" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C421" s="1">
+        <v>20</v>
+      </c>
+      <c r="D421" s="1">
+        <v>0</v>
+      </c>
+      <c r="E421" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F421" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="422" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A422" s="1">
+        <v>3</v>
+      </c>
+      <c r="B422" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C422" s="1">
+        <v>1</v>
+      </c>
+      <c r="D422" s="1">
+        <v>0</v>
+      </c>
+      <c r="E422" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F422" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="423" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A423" s="1">
+        <v>3</v>
+      </c>
+      <c r="B423" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C423" s="1">
+        <v>2</v>
+      </c>
+      <c r="D423" s="1">
+        <v>0</v>
+      </c>
+      <c r="E423" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F423" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="424" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A424" s="1">
+        <v>3</v>
+      </c>
+      <c r="B424" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C424" s="1">
+        <v>3</v>
+      </c>
+      <c r="D424" s="1">
+        <v>0</v>
+      </c>
+      <c r="E424" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F424" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="425" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A425" s="1">
+        <v>3</v>
+      </c>
+      <c r="B425" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C425" s="1">
+        <v>4</v>
+      </c>
+      <c r="D425" s="1">
+        <v>0</v>
+      </c>
+      <c r="E425" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F425" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="426" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A426" s="1">
+        <v>3</v>
+      </c>
+      <c r="B426" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C426" s="1">
+        <v>5</v>
+      </c>
+      <c r="D426" s="1">
+        <v>0</v>
+      </c>
+      <c r="E426" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F426" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="427" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A427" s="1">
+        <v>3</v>
+      </c>
+      <c r="B427" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C427" s="1">
+        <v>6</v>
+      </c>
+      <c r="D427" s="1">
+        <v>0</v>
+      </c>
+      <c r="E427" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F427" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="428" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A428" s="1">
+        <v>3</v>
+      </c>
+      <c r="B428" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C428" s="1">
+        <v>7</v>
+      </c>
+      <c r="D428" s="1">
+        <v>0</v>
+      </c>
+      <c r="E428" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F428" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="429" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A429" s="1">
+        <v>3</v>
+      </c>
+      <c r="B429" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C429" s="1">
+        <v>8</v>
+      </c>
+      <c r="D429" s="1">
+        <v>0</v>
+      </c>
+      <c r="E429" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F429" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="430" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A430" s="1">
+        <v>3</v>
+      </c>
+      <c r="B430" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C430" s="1">
+        <v>9</v>
+      </c>
+      <c r="D430" s="1">
+        <v>0</v>
+      </c>
+      <c r="E430" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F430" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="431" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A431" s="1">
+        <v>3</v>
+      </c>
+      <c r="B431" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C431" s="1">
+        <v>10</v>
+      </c>
+      <c r="D431" s="1">
+        <v>0</v>
+      </c>
+      <c r="E431" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F431" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="432" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A432" s="1">
+        <v>3</v>
+      </c>
+      <c r="B432" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C432" s="1">
+        <v>11</v>
+      </c>
+      <c r="D432" s="1">
+        <v>0</v>
+      </c>
+      <c r="E432" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F432" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="433" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A433" s="1">
+        <v>3</v>
+      </c>
+      <c r="B433" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C433" s="1">
+        <v>12</v>
+      </c>
+      <c r="D433" s="1">
+        <v>1</v>
+      </c>
+      <c r="E433" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F433" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="434" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A434" s="1">
+        <v>3</v>
+      </c>
+      <c r="B434" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C434" s="1">
+        <v>13</v>
+      </c>
+      <c r="D434" s="1">
+        <v>0</v>
+      </c>
+      <c r="E434" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F434" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="435" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A435" s="1">
+        <v>3</v>
+      </c>
+      <c r="B435" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C435" s="1">
+        <v>14</v>
+      </c>
+      <c r="D435" s="1">
+        <v>0</v>
+      </c>
+      <c r="E435" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F435" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="436" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A436" s="1">
+        <v>3</v>
+      </c>
+      <c r="B436" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C436" s="1">
+        <v>15</v>
+      </c>
+      <c r="D436" s="1">
+        <v>0</v>
+      </c>
+      <c r="E436" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F436" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="437" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A437" s="1">
+        <v>3</v>
+      </c>
+      <c r="B437" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C437" s="1">
+        <v>16</v>
+      </c>
+      <c r="D437" s="1">
+        <v>0</v>
+      </c>
+      <c r="E437" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F437" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="438" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A438" s="1">
+        <v>3</v>
+      </c>
+      <c r="B438" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C438" s="1">
+        <v>17</v>
+      </c>
+      <c r="D438" s="1">
+        <v>0</v>
+      </c>
+      <c r="E438" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F438" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="439" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A439" s="1">
+        <v>3</v>
+      </c>
+      <c r="B439" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C439" s="1">
+        <v>18</v>
+      </c>
+      <c r="D439" s="1">
+        <v>0</v>
+      </c>
+      <c r="E439" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F439" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="440" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A440" s="1">
+        <v>3</v>
+      </c>
+      <c r="B440" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C440" s="1">
+        <v>19</v>
+      </c>
+      <c r="D440" s="1">
+        <v>0</v>
+      </c>
+      <c r="E440" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F440" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="441" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A441" s="1">
+        <v>3</v>
+      </c>
+      <c r="B441" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C441" s="1">
+        <v>20</v>
+      </c>
+      <c r="D441" s="1">
+        <v>0</v>
+      </c>
+      <c r="E441" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F441" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="442" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A442" s="4">
+        <v>3</v>
+      </c>
+      <c r="B442" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C442" s="4">
+        <v>1</v>
+      </c>
+      <c r="D442" s="4">
+        <v>0</v>
+      </c>
+      <c r="E442" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F442" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="443" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A443" s="4">
+        <v>3</v>
+      </c>
+      <c r="B443" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C443" s="4">
+        <v>2</v>
+      </c>
+      <c r="D443" s="4">
+        <v>1</v>
+      </c>
+      <c r="E443" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F443" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="444" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A444" s="4">
+        <v>3</v>
+      </c>
+      <c r="B444" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C444" s="4">
+        <v>3</v>
+      </c>
+      <c r="D444" s="4">
+        <v>0</v>
+      </c>
+      <c r="E444" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F444" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="445" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A445" s="4">
+        <v>3</v>
+      </c>
+      <c r="B445" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C445" s="4">
+        <v>4</v>
+      </c>
+      <c r="D445" s="4">
+        <v>0</v>
+      </c>
+      <c r="E445" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F445" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="446" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A446" s="4">
+        <v>3</v>
+      </c>
+      <c r="B446" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C446" s="4">
+        <v>5</v>
+      </c>
+      <c r="D446" s="4">
+        <v>0</v>
+      </c>
+      <c r="E446" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F446" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="447" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A447" s="4">
+        <v>3</v>
+      </c>
+      <c r="B447" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C447" s="4">
+        <v>6</v>
+      </c>
+      <c r="D447" s="4">
+        <v>0</v>
+      </c>
+      <c r="E447" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F447" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="448" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A448" s="4">
+        <v>3</v>
+      </c>
+      <c r="B448" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C448" s="4">
+        <v>7</v>
+      </c>
+      <c r="D448" s="4">
+        <v>0</v>
+      </c>
+      <c r="E448" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F448" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="449" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A449" s="4">
+        <v>3</v>
+      </c>
+      <c r="B449" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C449" s="4">
+        <v>8</v>
+      </c>
+      <c r="D449" s="4">
+        <v>0</v>
+      </c>
+      <c r="E449" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F449" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="450" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A450" s="4">
+        <v>3</v>
+      </c>
+      <c r="B450" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C450" s="4">
+        <v>9</v>
+      </c>
+      <c r="D450" s="4">
+        <v>0</v>
+      </c>
+      <c r="E450" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F450" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="451" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A451" s="4">
+        <v>3</v>
+      </c>
+      <c r="B451" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C451" s="4">
+        <v>10</v>
+      </c>
+      <c r="D451" s="4">
+        <v>0</v>
+      </c>
+      <c r="E451" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F451" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="452" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A452" s="4">
+        <v>3</v>
+      </c>
+      <c r="B452" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C452" s="4">
+        <v>11</v>
+      </c>
+      <c r="D452" s="4">
+        <v>0</v>
+      </c>
+      <c r="E452" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F452" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="453" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A453" s="4">
+        <v>3</v>
+      </c>
+      <c r="B453" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C453" s="4">
+        <v>12</v>
+      </c>
+      <c r="D453" s="4">
+        <v>0</v>
+      </c>
+      <c r="E453" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F453" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="454" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A454" s="4">
+        <v>3</v>
+      </c>
+      <c r="B454" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C454" s="4">
+        <v>13</v>
+      </c>
+      <c r="D454" s="4">
+        <v>0</v>
+      </c>
+      <c r="E454" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F454" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="455" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A455" s="4">
+        <v>3</v>
+      </c>
+      <c r="B455" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C455" s="4">
+        <v>14</v>
+      </c>
+      <c r="D455" s="4">
+        <v>0</v>
+      </c>
+      <c r="E455" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F455" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="456" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A456" s="4">
+        <v>3</v>
+      </c>
+      <c r="B456" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C456" s="4">
+        <v>15</v>
+      </c>
+      <c r="D456" s="4">
+        <v>0</v>
+      </c>
+      <c r="E456" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F456" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="457" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A457" s="4">
+        <v>3</v>
+      </c>
+      <c r="B457" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C457" s="4">
+        <v>16</v>
+      </c>
+      <c r="D457" s="4">
+        <v>0</v>
+      </c>
+      <c r="E457" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F457" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="458" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A458" s="4">
+        <v>3</v>
+      </c>
+      <c r="B458" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C458" s="4">
+        <v>17</v>
+      </c>
+      <c r="D458" s="4">
+        <v>0</v>
+      </c>
+      <c r="E458" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F458" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="459" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A459" s="4">
+        <v>3</v>
+      </c>
+      <c r="B459" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C459" s="4">
+        <v>18</v>
+      </c>
+      <c r="D459" s="4">
+        <v>0</v>
+      </c>
+      <c r="E459" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F459" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="460" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A460" s="4">
+        <v>3</v>
+      </c>
+      <c r="B460" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C460" s="4">
+        <v>19</v>
+      </c>
+      <c r="D460" s="4">
+        <v>0</v>
+      </c>
+      <c r="E460" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F460" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="461" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A461" s="4">
+        <v>3</v>
+      </c>
+      <c r="B461" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C461" s="4">
+        <v>20</v>
+      </c>
+      <c r="D461" s="4">
+        <v>0</v>
+      </c>
+      <c r="E461" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F461" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="462" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A462" s="4">
+        <v>3</v>
+      </c>
+      <c r="B462" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C462" s="4">
+        <v>1</v>
+      </c>
+      <c r="D462" s="4">
+        <v>0</v>
+      </c>
+      <c r="E462" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F462" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="463" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A463" s="4">
+        <v>3</v>
+      </c>
+      <c r="B463" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C463" s="4">
+        <v>2</v>
+      </c>
+      <c r="D463" s="4">
+        <v>0</v>
+      </c>
+      <c r="E463" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F463" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="464" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A464" s="4">
+        <v>3</v>
+      </c>
+      <c r="B464" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C464" s="4">
+        <v>3</v>
+      </c>
+      <c r="D464" s="4">
+        <v>0</v>
+      </c>
+      <c r="E464" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F464" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="465" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A465" s="4">
+        <v>3</v>
+      </c>
+      <c r="B465" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C465" s="4">
+        <v>4</v>
+      </c>
+      <c r="D465" s="4">
+        <v>0</v>
+      </c>
+      <c r="E465" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F465" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="466" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A466" s="4">
+        <v>3</v>
+      </c>
+      <c r="B466" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C466" s="4">
+        <v>5</v>
+      </c>
+      <c r="D466" s="4">
+        <v>0</v>
+      </c>
+      <c r="E466" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F466" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="467" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A467" s="4">
+        <v>3</v>
+      </c>
+      <c r="B467" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C467" s="4">
+        <v>6</v>
+      </c>
+      <c r="D467" s="4">
+        <v>0</v>
+      </c>
+      <c r="E467" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F467" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="468" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A468" s="4">
+        <v>3</v>
+      </c>
+      <c r="B468" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C468" s="4">
+        <v>7</v>
+      </c>
+      <c r="D468" s="4">
+        <v>0</v>
+      </c>
+      <c r="E468" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F468" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="469" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A469" s="4">
+        <v>3</v>
+      </c>
+      <c r="B469" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C469" s="4">
+        <v>8</v>
+      </c>
+      <c r="D469" s="4">
+        <v>0</v>
+      </c>
+      <c r="E469" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F469" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="470" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A470" s="4">
+        <v>3</v>
+      </c>
+      <c r="B470" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C470" s="4">
+        <v>9</v>
+      </c>
+      <c r="D470" s="4">
+        <v>0</v>
+      </c>
+      <c r="E470" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F470" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="471" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A471" s="4">
+        <v>3</v>
+      </c>
+      <c r="B471" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C471" s="4">
+        <v>10</v>
+      </c>
+      <c r="D471" s="4">
+        <v>0</v>
+      </c>
+      <c r="E471" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F471" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="472" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A472" s="4">
+        <v>3</v>
+      </c>
+      <c r="B472" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C472" s="4">
+        <v>11</v>
+      </c>
+      <c r="D472" s="4">
+        <v>0</v>
+      </c>
+      <c r="E472" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F472" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="473" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A473" s="4">
+        <v>3</v>
+      </c>
+      <c r="B473" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C473" s="4">
+        <v>12</v>
+      </c>
+      <c r="D473" s="4">
+        <v>0</v>
+      </c>
+      <c r="E473" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F473" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="474" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A474" s="4">
+        <v>3</v>
+      </c>
+      <c r="B474" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C474" s="4">
+        <v>13</v>
+      </c>
+      <c r="D474" s="4">
+        <v>0</v>
+      </c>
+      <c r="E474" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F474" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="475" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A475" s="4">
+        <v>3</v>
+      </c>
+      <c r="B475" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C475" s="4">
+        <v>14</v>
+      </c>
+      <c r="D475" s="4">
+        <v>0</v>
+      </c>
+      <c r="E475" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F475" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="476" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A476" s="4">
+        <v>3</v>
+      </c>
+      <c r="B476" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C476" s="4">
+        <v>15</v>
+      </c>
+      <c r="D476" s="4">
+        <v>0</v>
+      </c>
+      <c r="E476" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F476" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="477" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A477" s="4">
+        <v>3</v>
+      </c>
+      <c r="B477" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C477" s="4">
+        <v>16</v>
+      </c>
+      <c r="D477" s="4">
+        <v>0</v>
+      </c>
+      <c r="E477" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F477" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="478" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A478" s="4">
+        <v>3</v>
+      </c>
+      <c r="B478" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C478" s="4">
+        <v>17</v>
+      </c>
+      <c r="D478" s="4">
+        <v>0</v>
+      </c>
+      <c r="E478" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F478" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="479" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A479" s="4">
+        <v>3</v>
+      </c>
+      <c r="B479" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C479" s="4">
+        <v>18</v>
+      </c>
+      <c r="D479" s="4">
+        <v>0</v>
+      </c>
+      <c r="E479" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F479" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="480" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A480" s="4">
+        <v>3</v>
+      </c>
+      <c r="B480" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C480" s="4">
+        <v>19</v>
+      </c>
+      <c r="D480" s="4">
+        <v>0</v>
+      </c>
+      <c r="E480" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F480" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="481" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A481" s="4">
+        <v>3</v>
+      </c>
+      <c r="B481" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C481" s="4">
+        <v>20</v>
+      </c>
+      <c r="D481" s="4">
+        <v>0</v>
+      </c>
+      <c r="E481" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F481" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="482" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A482" s="4">
+        <v>3</v>
+      </c>
+      <c r="B482" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C482" s="4">
+        <v>1</v>
+      </c>
+      <c r="D482" s="4">
+        <v>0</v>
+      </c>
+      <c r="E482" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F482" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="483" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A483" s="4">
+        <v>3</v>
+      </c>
+      <c r="B483" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C483" s="4">
+        <v>2</v>
+      </c>
+      <c r="D483" s="4">
+        <v>1</v>
+      </c>
+      <c r="E483" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F483" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="484" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A484" s="4">
+        <v>3</v>
+      </c>
+      <c r="B484" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C484" s="4">
+        <v>3</v>
+      </c>
+      <c r="D484" s="4">
+        <v>0</v>
+      </c>
+      <c r="E484" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F484" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="485" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A485" s="4">
+        <v>3</v>
+      </c>
+      <c r="B485" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C485" s="4">
+        <v>4</v>
+      </c>
+      <c r="D485" s="4">
+        <v>0</v>
+      </c>
+      <c r="E485" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F485" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="486" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A486" s="4">
+        <v>3</v>
+      </c>
+      <c r="B486" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C486" s="4">
+        <v>5</v>
+      </c>
+      <c r="D486" s="4">
+        <v>0</v>
+      </c>
+      <c r="E486" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F486" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="487" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A487" s="4">
+        <v>3</v>
+      </c>
+      <c r="B487" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C487" s="4">
+        <v>6</v>
+      </c>
+      <c r="D487" s="4">
+        <v>0</v>
+      </c>
+      <c r="E487" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F487" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="488" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A488" s="4">
+        <v>3</v>
+      </c>
+      <c r="B488" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C488" s="4">
+        <v>7</v>
+      </c>
+      <c r="D488" s="4">
+        <v>0</v>
+      </c>
+      <c r="E488" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F488" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="489" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A489" s="4">
+        <v>3</v>
+      </c>
+      <c r="B489" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C489" s="4">
+        <v>8</v>
+      </c>
+      <c r="D489" s="4">
+        <v>0</v>
+      </c>
+      <c r="E489" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F489" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="490" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A490" s="4">
+        <v>3</v>
+      </c>
+      <c r="B490" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C490" s="4">
+        <v>9</v>
+      </c>
+      <c r="D490" s="4">
+        <v>0</v>
+      </c>
+      <c r="E490" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F490" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="491" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A491" s="4">
+        <v>3</v>
+      </c>
+      <c r="B491" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C491" s="4">
+        <v>10</v>
+      </c>
+      <c r="D491" s="4">
+        <v>0</v>
+      </c>
+      <c r="E491" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F491" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="492" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A492" s="4">
+        <v>3</v>
+      </c>
+      <c r="B492" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C492" s="4">
+        <v>11</v>
+      </c>
+      <c r="D492" s="4">
+        <v>0</v>
+      </c>
+      <c r="E492" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F492" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="493" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A493" s="4">
+        <v>3</v>
+      </c>
+      <c r="B493" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C493" s="4">
+        <v>12</v>
+      </c>
+      <c r="D493" s="4">
+        <v>0</v>
+      </c>
+      <c r="E493" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F493" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="494" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A494" s="4">
+        <v>3</v>
+      </c>
+      <c r="B494" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C494" s="4">
+        <v>13</v>
+      </c>
+      <c r="D494" s="4">
+        <v>0</v>
+      </c>
+      <c r="E494" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F494" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="495" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A495" s="4">
+        <v>3</v>
+      </c>
+      <c r="B495" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C495" s="4">
+        <v>14</v>
+      </c>
+      <c r="D495" s="4">
+        <v>0</v>
+      </c>
+      <c r="E495" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F495" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="496" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A496" s="4">
+        <v>3</v>
+      </c>
+      <c r="B496" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C496" s="4">
+        <v>15</v>
+      </c>
+      <c r="D496" s="4">
+        <v>0</v>
+      </c>
+      <c r="E496" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F496" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="497" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A497" s="4">
+        <v>3</v>
+      </c>
+      <c r="B497" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C497" s="4">
+        <v>16</v>
+      </c>
+      <c r="D497" s="4">
+        <v>0</v>
+      </c>
+      <c r="E497" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F497" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="498" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A498" s="4">
+        <v>3</v>
+      </c>
+      <c r="B498" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C498" s="4">
+        <v>17</v>
+      </c>
+      <c r="D498" s="4">
+        <v>0</v>
+      </c>
+      <c r="E498" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F498" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="499" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A499" s="4">
+        <v>3</v>
+      </c>
+      <c r="B499" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C499" s="4">
+        <v>18</v>
+      </c>
+      <c r="D499" s="4">
+        <v>0</v>
+      </c>
+      <c r="E499" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F499" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="500" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A500" s="4">
+        <v>3</v>
+      </c>
+      <c r="B500" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C500" s="4">
+        <v>19</v>
+      </c>
+      <c r="D500" s="4">
+        <v>0</v>
+      </c>
+      <c r="E500" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F500" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="501" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A501" s="4">
+        <v>3</v>
+      </c>
+      <c r="B501" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C501" s="4">
+        <v>20</v>
+      </c>
+      <c r="D501" s="4">
+        <v>0</v>
+      </c>
+      <c r="E501" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F501" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="502" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A502" s="4">
+        <v>3</v>
+      </c>
+      <c r="B502" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C502" s="4">
+        <v>1</v>
+      </c>
+      <c r="D502" s="4">
+        <v>0</v>
+      </c>
+      <c r="E502" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F502" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="503" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A503" s="4">
+        <v>3</v>
+      </c>
+      <c r="B503" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C503" s="4">
+        <v>2</v>
+      </c>
+      <c r="D503" s="4">
+        <v>0</v>
+      </c>
+      <c r="E503" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F503" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="504" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A504" s="4">
+        <v>3</v>
+      </c>
+      <c r="B504" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C504" s="4">
+        <v>3</v>
+      </c>
+      <c r="D504" s="4">
+        <v>0</v>
+      </c>
+      <c r="E504" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F504" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="505" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A505" s="4">
+        <v>3</v>
+      </c>
+      <c r="B505" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C505" s="4">
+        <v>4</v>
+      </c>
+      <c r="D505" s="4">
+        <v>0</v>
+      </c>
+      <c r="E505" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F505" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="506" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A506" s="4">
+        <v>3</v>
+      </c>
+      <c r="B506" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C506" s="4">
+        <v>5</v>
+      </c>
+      <c r="D506" s="4">
+        <v>0</v>
+      </c>
+      <c r="E506" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F506" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="507" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A507" s="4">
+        <v>3</v>
+      </c>
+      <c r="B507" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C507" s="4">
+        <v>6</v>
+      </c>
+      <c r="D507" s="4">
+        <v>0</v>
+      </c>
+      <c r="E507" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F507" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="508" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A508" s="4">
+        <v>3</v>
+      </c>
+      <c r="B508" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C508" s="4">
+        <v>7</v>
+      </c>
+      <c r="D508" s="4">
+        <v>0</v>
+      </c>
+      <c r="E508" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F508" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="509" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A509" s="4">
+        <v>3</v>
+      </c>
+      <c r="B509" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C509" s="4">
+        <v>8</v>
+      </c>
+      <c r="D509" s="4">
+        <v>0</v>
+      </c>
+      <c r="E509" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F509" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="510" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A510" s="4">
+        <v>3</v>
+      </c>
+      <c r="B510" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C510" s="4">
+        <v>9</v>
+      </c>
+      <c r="D510" s="4">
+        <v>0</v>
+      </c>
+      <c r="E510" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F510" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="511" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A511" s="4">
+        <v>3</v>
+      </c>
+      <c r="B511" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C511" s="4">
+        <v>10</v>
+      </c>
+      <c r="D511" s="4">
+        <v>0</v>
+      </c>
+      <c r="E511" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F511" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="512" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A512" s="4">
+        <v>3</v>
+      </c>
+      <c r="B512" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C512" s="4">
+        <v>11</v>
+      </c>
+      <c r="D512" s="4">
+        <v>0</v>
+      </c>
+      <c r="E512" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F512" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="513" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A513" s="4">
+        <v>3</v>
+      </c>
+      <c r="B513" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C513" s="4">
+        <v>12</v>
+      </c>
+      <c r="D513" s="4">
+        <v>0</v>
+      </c>
+      <c r="E513" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F513" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="514" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A514" s="4">
+        <v>3</v>
+      </c>
+      <c r="B514" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C514" s="4">
+        <v>13</v>
+      </c>
+      <c r="D514" s="4">
+        <v>0</v>
+      </c>
+      <c r="E514" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F514" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="515" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A515" s="4">
+        <v>3</v>
+      </c>
+      <c r="B515" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C515" s="4">
+        <v>14</v>
+      </c>
+      <c r="D515" s="4">
+        <v>0</v>
+      </c>
+      <c r="E515" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F515" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="516" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A516" s="4">
+        <v>3</v>
+      </c>
+      <c r="B516" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C516" s="4">
+        <v>15</v>
+      </c>
+      <c r="D516" s="4">
+        <v>0</v>
+      </c>
+      <c r="E516" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F516" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="517" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A517" s="4">
+        <v>3</v>
+      </c>
+      <c r="B517" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C517" s="4">
+        <v>16</v>
+      </c>
+      <c r="D517" s="4">
+        <v>1</v>
+      </c>
+      <c r="E517" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F517" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="518" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A518" s="4">
+        <v>3</v>
+      </c>
+      <c r="B518" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C518" s="4">
+        <v>17</v>
+      </c>
+      <c r="D518" s="4">
+        <v>0</v>
+      </c>
+      <c r="E518" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F518" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="519" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A519" s="4">
+        <v>3</v>
+      </c>
+      <c r="B519" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C519" s="4">
+        <v>18</v>
+      </c>
+      <c r="D519" s="4">
+        <v>0</v>
+      </c>
+      <c r="E519" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F519" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="520" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A520" s="4">
+        <v>3</v>
+      </c>
+      <c r="B520" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C520" s="4">
+        <v>19</v>
+      </c>
+      <c r="D520" s="4">
+        <v>0</v>
+      </c>
+      <c r="E520" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F520" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="521" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A521" s="4">
+        <v>3</v>
+      </c>
+      <c r="B521" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C521" s="4">
+        <v>20</v>
+      </c>
+      <c r="D521" s="4">
+        <v>0</v>
+      </c>
+      <c r="E521" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F521" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8114,7 +11376,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8415,10 +11677,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8517,6 +11779,14 @@
       </c>
       <c r="B12" s="1" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -8529,15 +11799,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
@@ -8545,7 +11815,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -8559,6 +11829,14 @@
       </c>
       <c r="B3">
         <v>2017</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2018</v>
       </c>
     </row>
   </sheetData>
@@ -8573,13 +11851,13 @@
   </sheetPr>
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
@@ -8590,7 +11868,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -8601,7 +11879,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -8612,7 +11890,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -8623,7 +11901,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -8634,7 +11912,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -8645,7 +11923,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -8656,7 +11934,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -8667,7 +11945,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -8678,7 +11956,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -8689,7 +11967,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -8700,7 +11978,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -8711,7 +11989,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -8722,7 +12000,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>1</v>
       </c>
@@ -8733,7 +12011,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>1</v>
       </c>
@@ -8744,7 +12022,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>1</v>
       </c>
@@ -8755,7 +12033,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>1</v>
       </c>
@@ -8766,7 +12044,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>1</v>
       </c>
@@ -8777,7 +12055,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>1</v>
       </c>
@@ -8788,7 +12066,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>1</v>
       </c>
@@ -8799,7 +12077,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>1</v>
       </c>
@@ -8810,7 +12088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>1</v>
       </c>

</xml_diff>